<commit_message>
change culture name to replace spaces
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Niek/Library/Mobile Documents/com~apple~CloudDocs/code/plotting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE7DAB-52FF-D349-B188-B7E54D96FF22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F38218-F581-6540-9734-152CA0128C17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="15760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,12 +57,6 @@
     <t>substrate_ppm</t>
   </si>
   <si>
-    <t>culture 1</t>
-  </si>
-  <si>
-    <t>culture 2</t>
-  </si>
-  <si>
     <t>control</t>
   </si>
   <si>
@@ -73,6 +67,12 @@
   </si>
   <si>
     <t>productC_uM</t>
+  </si>
+  <si>
+    <t>culture_1</t>
+  </si>
+  <si>
+    <t>culture_2</t>
   </si>
 </sst>
 </file>
@@ -414,13 +414,13 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -437,7 +437,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
         <v>43448</v>
@@ -472,7 +472,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>43454</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>43468</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>43486</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>43496</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
         <v>43511</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>43518</v>
@@ -682,7 +682,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>43532</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>43532</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>43539</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>43546</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1">
         <v>43552</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>43448</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>43454</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1">
         <v>43468</v>
@@ -962,7 +962,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
         <v>43486</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1">
         <v>43486</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1">
         <v>43496</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B20" s="1">
         <v>43511</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B21" s="1">
         <v>43518</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
         <v>43518</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B23" s="1">
         <v>43532</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1">
         <v>43539</v>
@@ -1242,7 +1242,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1">
         <v>43546</v>
@@ -1277,7 +1277,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1">
         <v>43552</v>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B27" s="1">
         <v>43448</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B28" s="1">
         <v>43454</v>
@@ -1382,7 +1382,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1">
         <v>43468</v>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1">
         <v>43486</v>
@@ -1452,7 +1452,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1">
         <v>43496</v>
@@ -1487,7 +1487,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B32" s="1">
         <v>43511</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B33" s="1">
         <v>43518</v>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B34" s="1">
         <v>43532</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B35" s="1">
         <v>43539</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B36" s="1">
         <v>43546</v>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B37" s="1">
         <v>43552</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B38" s="1">
         <v>43560</v>

</xml_diff>